<commit_message>
added fixes to lesson 6
</commit_message>
<xml_diff>
--- a/dkoltovich/lesson_6/data.xlsx
+++ b/dkoltovich/lesson_6/data.xlsx
@@ -536,32 +536,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>875-70-37</t>
+          <t>500-23-12</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>749-74-33</t>
+          <t>142-96-12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>845-88-46</t>
+          <t>915-87-44</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>501-39-60</t>
+          <t>967-72-31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>806-53-75</t>
+          <t>944-88-25</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>654-76-23</t>
+          <t>766-43-43</t>
         </is>
       </c>
     </row>

</xml_diff>